<commit_message>
feat: Actualizar Cádiz + añadir PDF adjunto
- Cádiz.xlsx actualizado con envíos iniciados
- Añadido PDF "Equipamiento Astroturismo 2026.pdf"
- Almería completado: 63/64 enviados

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/provincias/Cadiz.xlsx
+++ b/provincias/Cadiz.xlsx
@@ -503,7 +503,11 @@
           <t>https://www.todoslosayuntamientos.es/andalucia/cadiz/setenil-de-las-bodegas</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2026-01-20 08:25</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">

</xml_diff>